<commit_message>
started data analysis of 4C8 shouldnt actually take too long
</commit_message>
<xml_diff>
--- a/IIB/4C8/data.xlsx
+++ b/IIB/4C8/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIB\4C8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30B7BBC-D5E4-49D4-8DBF-C662C31BB2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4C79B-9737-4BEA-A100-A27ECD483DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{BB3B62A8-AAC0-40D0-8333-654D43E65E71}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{BB3B62A8-AAC0-40D0-8333-654D43E65E71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="24">
   <si>
     <t>cal</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>mass (kg)</t>
+  </si>
+  <si>
+    <t>xi</t>
   </si>
 </sst>
 </file>
@@ -596,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE8DC6C-CFC9-4DD6-ACDA-CD2B09895C7F}">
   <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -746,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB46CFC6-DD2E-48F9-9340-A4BF4784A7AC}">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -812,6 +815,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -820,7 +824,7 @@
   <dimension ref="B1:J46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -919,7 +923,20 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <f>(C5-C4)/((C6-C4)+(C6-C5))</f>
+        <v>4.2435424354243537E-2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <f>(H5-H4)/((H6-H4)+(H6-H5))</f>
+        <v>3.6199095022624368E-2</v>
+      </c>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.45">
@@ -989,9 +1006,7 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="2"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.45">
@@ -1079,9 +1094,21 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <f>(C16-C15)/((C17-C15)+(C17-C16))</f>
+        <v>9.5823095823095852E-2</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18">
+        <f>(H16-H15)/((H17-H15)+(H17-H16))</f>
+        <v>5.4973821989528784E-2</v>
+      </c>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.45">
@@ -1249,11 +1276,21 @@
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
+      <c r="B30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <f>(C28-C27)/((C29-C27)+(C29-C28))</f>
+        <v>0.15000000000000008</v>
+      </c>
       <c r="E30" s="3"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
+      <c r="G30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <f>(H28-H27)/((H29-H27)+(H29-H28))</f>
+        <v>7.7452667814113543E-2</v>
+      </c>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.45">
@@ -1368,6 +1405,7 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1376,7 +1414,7 @@
   <dimension ref="B3:H26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1474,9 +1512,21 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <f>(C7-C6)/((C8-C6)+(C8-C7))</f>
+        <v>5.9063136456211821E-2</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <f>(G7-G6)/((G8-G6)+(G8-G7))</f>
+        <v>8.604206500956027E-2</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
@@ -1561,8 +1611,18 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="2"/>
+      <c r="C15">
+        <f>(C13-C12)/((C14-C12)+(C14-C13))</f>
+        <v>9.700598802395205E-2</v>
+      </c>
       <c r="D15" s="3"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <f>(G13-G12)/((G14-G12)+(G14-G13))</f>
+        <v>0.13701923076923084</v>
+      </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.45">
@@ -1650,9 +1710,21 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <f>(C20-C19)/((C21-C19)+(C21-C20))</f>
+        <v>0.1232</v>
+      </c>
       <c r="D22" s="3"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22">
+        <f>(G20-G19)/((G21-G19)+(G21-G20))</f>
+        <v>0.16271186440677968</v>
+      </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
progress with 4C8 moving forwards will get done by end of week am certain then weekend can be on 4F2 again horay i love 4f2
</commit_message>
<xml_diff>
--- a/IIB/4C8/data.xlsx
+++ b/IIB/4C8/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIB\4C8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4C79B-9737-4BEA-A100-A27ECD483DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D34850-ABCE-4409-AC9C-EF3F8A057975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{BB3B62A8-AAC0-40D0-8333-654D43E65E71}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{BB3B62A8-AAC0-40D0-8333-654D43E65E71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -749,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB46CFC6-DD2E-48F9-9340-A4BF4784A7AC}">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C08535-16F5-436C-8EC3-18DE79FDCF07}">
   <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>